<commit_message>
Changes Edgar scaling to use newer data files. Removes old data files.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Edgar_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Edgar_scaling_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="480" windowWidth="17720" windowHeight="12980" tabRatio="500"/>
+    <workbookView xWindow="-25000" yWindow="7480" windowWidth="17580" windowHeight="12940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -107,18 +107,9 @@
     <t>1A4c_Agriculture-forestry-fishing</t>
   </si>
   <si>
-    <t>1A5_Other-unspecified</t>
-  </si>
-  <si>
     <t>1B2_Fugitive-petr-and-gas</t>
   </si>
   <si>
-    <t>2A1_Cement-production</t>
-  </si>
-  <si>
-    <t>2A2_Lime-production</t>
-  </si>
-  <si>
     <t>2B_Chemical-industry</t>
   </si>
   <si>
@@ -128,87 +119,12 @@
     <t>1A3ai_International-aviation</t>
   </si>
   <si>
-    <t>1A1a1</t>
-  </si>
-  <si>
-    <t>1A1a2</t>
-  </si>
-  <si>
-    <t>1A1a5</t>
-  </si>
-  <si>
-    <t>1A1a6</t>
-  </si>
-  <si>
-    <t>1A1a7</t>
-  </si>
-  <si>
-    <t>1A1ax2</t>
-  </si>
-  <si>
-    <t>1A1ax4</t>
-  </si>
-  <si>
-    <t>1A1ax5</t>
-  </si>
-  <si>
-    <t>1A1ax6</t>
-  </si>
-  <si>
-    <t>1A1ax7</t>
-  </si>
-  <si>
-    <t>1A1b</t>
-  </si>
-  <si>
-    <t>1A1c1</t>
-  </si>
-  <si>
-    <t>1A1c5</t>
-  </si>
-  <si>
-    <t>1A2a</t>
-  </si>
-  <si>
-    <t>1A2ax</t>
-  </si>
-  <si>
-    <t>1A2b</t>
-  </si>
-  <si>
-    <t>1A2c</t>
-  </si>
-  <si>
-    <t>1A2d</t>
-  </si>
-  <si>
-    <t>1A2dx</t>
-  </si>
-  <si>
-    <t>1A2e</t>
-  </si>
-  <si>
-    <t>1A2f</t>
-  </si>
-  <si>
-    <t>1A2f1</t>
-  </si>
-  <si>
-    <t>1A2f2</t>
-  </si>
-  <si>
-    <t>1A2fx</t>
-  </si>
-  <si>
     <t>1A3a</t>
   </si>
   <si>
     <t>1A3b</t>
   </si>
   <si>
-    <t>1A3bx</t>
-  </si>
-  <si>
     <t>1A3c</t>
   </si>
   <si>
@@ -218,169 +134,106 @@
     <t>1A3e</t>
   </si>
   <si>
-    <t>1A4a</t>
-  </si>
-  <si>
-    <t>1A4ax</t>
-  </si>
-  <si>
-    <t>1A4b</t>
-  </si>
-  <si>
-    <t>1A4bx</t>
-  </si>
-  <si>
-    <t>1A4c1</t>
-  </si>
-  <si>
-    <t>1A4c1x</t>
-  </si>
-  <si>
-    <t>1A4c2</t>
-  </si>
-  <si>
-    <t>1A4d</t>
-  </si>
-  <si>
-    <t>1B2c</t>
-  </si>
-  <si>
-    <t>2B5a</t>
-  </si>
-  <si>
-    <t>2B5g</t>
-  </si>
-  <si>
-    <t>2C2</t>
-  </si>
-  <si>
-    <t>2C3a</t>
-  </si>
-  <si>
-    <t>2C5cp</t>
-  </si>
-  <si>
-    <t>2C5cs</t>
-  </si>
-  <si>
-    <t>2C5lp</t>
-  </si>
-  <si>
-    <t>2C5ls</t>
-  </si>
-  <si>
-    <t>2C5zp</t>
-  </si>
-  <si>
-    <t>6Cax</t>
-  </si>
-  <si>
-    <t>6Cb1</t>
-  </si>
-  <si>
-    <t>6Cb2</t>
-  </si>
-  <si>
-    <t>1A4dx</t>
-  </si>
-  <si>
-    <t>1A1a3</t>
-  </si>
-  <si>
-    <t>1A1ax1</t>
-  </si>
-  <si>
-    <t>1A1c2</t>
-  </si>
-  <si>
-    <t>1A1c3</t>
-  </si>
-  <si>
-    <t>1A2cx</t>
-  </si>
-  <si>
-    <t>1A2ex</t>
-  </si>
-  <si>
-    <t>1A3cx</t>
-  </si>
-  <si>
-    <t>1A3ex</t>
-  </si>
-  <si>
-    <t>2B5g2</t>
-  </si>
-  <si>
-    <t>2C5zs</t>
-  </si>
-  <si>
-    <t>7A1</t>
-  </si>
-  <si>
-    <t>1A1a4</t>
-  </si>
-  <si>
-    <t>1A1cx5</t>
-  </si>
-  <si>
-    <t>1A2bx</t>
-  </si>
-  <si>
-    <t>1A3dx</t>
-  </si>
-  <si>
-    <t>1A4c3</t>
-  </si>
-  <si>
-    <t>1A4c3x</t>
-  </si>
-  <si>
-    <t>1A5b1</t>
-  </si>
-  <si>
-    <t>1A1ax3</t>
-  </si>
-  <si>
-    <t>1A1bx</t>
-  </si>
-  <si>
-    <t>2A1</t>
-  </si>
-  <si>
-    <t>2A4a</t>
-  </si>
-  <si>
-    <t>2A2</t>
-  </si>
-  <si>
-    <t>1A1cx3</t>
-  </si>
-  <si>
-    <t>1A1cx4</t>
-  </si>
-  <si>
-    <t>7A2</t>
-  </si>
-  <si>
     <t>1C2</t>
   </si>
   <si>
-    <t>1C2x</t>
-  </si>
-  <si>
     <t>1C1</t>
   </si>
   <si>
     <t>1A2c_Ind-Comb-Chemicals</t>
   </si>
   <si>
-    <t>1A3a_aviation</t>
-  </si>
-  <si>
-    <t>1A3d_shipping</t>
-  </si>
-  <si>
     <t>7A_Fossil-fuel-fires</t>
+  </si>
+  <si>
+    <t>1A1a</t>
+  </si>
+  <si>
+    <t>1A1bc</t>
+  </si>
+  <si>
+    <t>1A2</t>
+  </si>
+  <si>
+    <t>1A4</t>
+  </si>
+  <si>
+    <t>1B2</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>4F</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>5C</t>
+  </si>
+  <si>
+    <t>5D</t>
+  </si>
+  <si>
+    <t>6C</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-Construction</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-transpequip</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-machinery</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-mining-quarying</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-wood-products</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-textile-leather</t>
+  </si>
+  <si>
+    <t>1A2g_Ind-Comb-other</t>
+  </si>
+  <si>
+    <t>1B2d_Fugitive-other-energy</t>
+  </si>
+  <si>
+    <t>2H_Pulp-and-paper-food-beverage-wood</t>
+  </si>
+  <si>
+    <t>3F_Agricultural-residue-burning-on-fields</t>
+  </si>
+  <si>
+    <t>5C_Waste-incineration</t>
+  </si>
+  <si>
+    <t>other-in-total</t>
+  </si>
+  <si>
+    <t>6A_Other-in-total</t>
+  </si>
+  <si>
+    <t>11B_Forest-fires</t>
+  </si>
+  <si>
+    <t>11C_Other-natural</t>
   </si>
 </sst>
 </file>
@@ -436,8 +289,112 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -533,7 +490,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="195">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -579,6 +536,58 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -624,6 +633,58 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -953,16 +1014,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="27.1640625" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -978,29 +1040,26 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>87</v>
-      </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -1008,606 +1067,360 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>88</v>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>40</v>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>105</v>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>41</v>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>42</v>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>43</v>
       </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>44</v>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>106</v>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>48</v>
-      </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>49</v>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
+        <v>45</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>100</v>
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" t="s">
-        <v>10</v>
+        <v>46</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>65</v>
-      </c>
-      <c r="B48" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>71</v>
-      </c>
-      <c r="B54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>73</v>
-      </c>
-      <c r="B60" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>107</v>
-      </c>
-      <c r="B64" t="s">
-        <v>30</v>
-      </c>
-      <c r="C64" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>109</v>
-      </c>
-      <c r="B65" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>108</v>
-      </c>
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>74</v>
-      </c>
-      <c r="B67" t="s">
-        <v>32</v>
-      </c>
-      <c r="C67" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>75</v>
-      </c>
-      <c r="B68" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>95</v>
-      </c>
-      <c r="B69" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>76</v>
-      </c>
-      <c r="B70" t="s">
-        <v>33</v>
-      </c>
-      <c r="C70" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>78</v>
-      </c>
-      <c r="B72" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75" t="s">
-        <v>33</v>
-      </c>
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>82</v>
-      </c>
-      <c r="B76" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>96</v>
-      </c>
-      <c r="B77" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>97</v>
-      </c>
-      <c r="B81" t="s">
-        <v>119</v>
-      </c>
-      <c r="C81" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
-        <v>112</v>
-      </c>
-      <c r="B82" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="B83" t="s">
-        <v>59</v>
-      </c>
-      <c r="C83" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="B84" t="s">
-        <v>118</v>
-      </c>
-      <c r="C84" t="s">
-        <v>22</v>
-      </c>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="1"/>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:C84">

</xml_diff>

<commit_message>
Remove open burning and natural emissions
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Edgar_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Edgar_scaling_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25000" yWindow="7480" windowWidth="17580" windowHeight="12940" tabRatio="500"/>
+    <workbookView xWindow="3880" yWindow="960" windowWidth="24640" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>11C_Other-natural</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Don't include in CMIP6 data product</t>
   </si>
 </sst>
 </file>
@@ -289,8 +295,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="195">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -490,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="195">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -588,6 +600,9 @@
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -685,6 +700,9 @@
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1014,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1027,7 +1045,7 @@
     <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1037,8 +1055,11 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1049,7 +1070,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>41</v>
       </c>
@@ -1057,7 +1078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -1065,7 +1086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1076,7 +1097,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1087,7 +1108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>43</v>
       </c>
@@ -1095,7 +1116,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -1103,7 +1124,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="B9" t="s">
         <v>43</v>
       </c>
@@ -1111,7 +1132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -1119,7 +1140,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="B11" t="s">
         <v>43</v>
       </c>
@@ -1127,7 +1148,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="B12" t="s">
         <v>43</v>
       </c>
@@ -1135,7 +1156,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -1143,7 +1164,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="B14" t="s">
         <v>43</v>
       </c>
@@ -1151,7 +1172,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="B15" t="s">
         <v>43</v>
       </c>
@@ -1159,7 +1180,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="B16" t="s">
         <v>43</v>
       </c>
@@ -1328,7 +1349,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1339,7 +1360,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -1350,51 +1371,52 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>50</v>
       </c>
-      <c r="B35" t="s">
-        <v>50</v>
-      </c>
       <c r="C35" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="B36" s="1"/>
       <c r="C36" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>52</v>
       </c>
-      <c r="B37" t="s">
-        <v>52</v>
-      </c>
       <c r="C37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>53</v>
       </c>
-      <c r="B38" t="s">
-        <v>53</v>
-      </c>
       <c r="C38" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -1405,7 +1427,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Change EDGAR scaling to only scale between 1992 and 2009 to avoid discontinuities due to different driver data assumptions.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/Edgar_scaling_mapping.xlsx
+++ b/input/mappings/scaling/Edgar_scaling_mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="174">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -447,12 +447,6 @@
   </si>
   <si>
     <t>mkd</t>
-  </si>
-  <si>
-    <t>idn</t>
-  </si>
-  <si>
-    <t>Eliminate jump in CO emissions present in EDGAR data</t>
   </si>
   <si>
     <t>Comment</t>
@@ -604,8 +598,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="401">
+  <cellStyleXfs count="405">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1015,7 +1013,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="401">
+  <cellStyles count="405">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1216,6 +1214,8 @@
     <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1416,6 +1416,8 @@
     <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1821,7 +1823,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1982,7 +1984,7 @@
         <v>115</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2051,7 +2053,7 @@
         <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2066,7 +2068,7 @@
         <v>27</v>
       </c>
       <c r="E29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2076,7 +2078,7 @@
         <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2106,7 +2108,7 @@
         <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2120,7 +2122,7 @@
         <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2134,7 +2136,7 @@
         <v>91</v>
       </c>
       <c r="E35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2148,7 +2150,7 @@
         <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2163,7 +2165,7 @@
         <v>28</v>
       </c>
       <c r="E37" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2177,7 +2179,7 @@
         <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2191,7 +2193,7 @@
         <v>63</v>
       </c>
       <c r="E39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2206,7 +2208,7 @@
         <v>84</v>
       </c>
       <c r="E40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2221,7 +2223,7 @@
         <v>82</v>
       </c>
       <c r="E41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2236,7 +2238,7 @@
         <v>85</v>
       </c>
       <c r="E42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2251,7 +2253,7 @@
         <v>83</v>
       </c>
       <c r="E43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2265,7 +2267,7 @@
         <v>101</v>
       </c>
       <c r="E44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2279,7 +2281,7 @@
         <v>94</v>
       </c>
       <c r="E45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2293,7 +2295,7 @@
         <v>99</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2308,7 +2310,7 @@
         <v>96</v>
       </c>
       <c r="E47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2322,7 +2324,7 @@
         <v>94</v>
       </c>
       <c r="E48" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2337,7 +2339,7 @@
         <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2413,7 +2415,7 @@
         <v>103</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2428,7 +2430,7 @@
         <v>77</v>
       </c>
       <c r="E57" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2442,7 +2444,7 @@
         <v>65</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2457,7 +2459,7 @@
         <v>75</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2592,11 +2594,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2627,15 +2629,15 @@
         <v>140</v>
       </c>
       <c r="H1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -2647,18 +2649,15 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <v>1990</v>
+        <v>1992</v>
       </c>
       <c r="G2">
-        <v>2010</v>
-      </c>
-      <c r="H2" t="s">
-        <v>143</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>137</v>
@@ -2676,10 +2675,10 @@
         <v>2000</v>
       </c>
       <c r="G3">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="H3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2696,7 +2695,7 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>1980</v>
+        <v>1992</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -2705,7 +2704,7 @@
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2722,7 +2721,7 @@
         <v>9</v>
       </c>
       <c r="E5">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -2731,7 +2730,7 @@
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2748,7 +2747,7 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -2757,12 +2756,12 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
         <v>137</v>
@@ -2774,7 +2773,7 @@
         <v>9</v>
       </c>
       <c r="E7">
-        <v>2010</v>
+        <v>1992</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -2783,12 +2782,12 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
         <v>137</v>
@@ -2799,22 +2798,22 @@
       <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8">
-        <v>1980</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8">
+        <v>1992</v>
+      </c>
+      <c r="G8">
+        <v>2009</v>
       </c>
       <c r="H8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
         <v>137</v>
@@ -2825,17 +2824,17 @@
       <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
         <v>1992</v>
       </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
+      <c r="G9">
+        <v>2009</v>
       </c>
       <c r="H9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2858,10 +2857,10 @@
         <v>1992</v>
       </c>
       <c r="G10">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2884,10 +2883,10 @@
         <v>1992</v>
       </c>
       <c r="G11">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2910,10 +2909,10 @@
         <v>1992</v>
       </c>
       <c r="G12">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2936,10 +2935,10 @@
         <v>1992</v>
       </c>
       <c r="G13">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2962,10 +2961,10 @@
         <v>1992</v>
       </c>
       <c r="G14">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2988,10 +2987,10 @@
         <v>1992</v>
       </c>
       <c r="G15">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -3014,10 +3013,10 @@
         <v>1992</v>
       </c>
       <c r="G16">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3040,10 +3039,10 @@
         <v>1992</v>
       </c>
       <c r="G17">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -3066,10 +3065,10 @@
         <v>1992</v>
       </c>
       <c r="G18">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -3092,10 +3091,10 @@
         <v>1992</v>
       </c>
       <c r="G19">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -3118,10 +3117,10 @@
         <v>1992</v>
       </c>
       <c r="G20">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -3144,10 +3143,10 @@
         <v>1992</v>
       </c>
       <c r="G21">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -3170,10 +3169,10 @@
         <v>1992</v>
       </c>
       <c r="G22">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3196,10 +3195,10 @@
         <v>1992</v>
       </c>
       <c r="G23">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H23" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3222,15 +3221,15 @@
         <v>1992</v>
       </c>
       <c r="G24">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H24" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B25" t="s">
         <v>137</v>
@@ -3248,15 +3247,15 @@
         <v>1992</v>
       </c>
       <c r="G25">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H25" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
         <v>137</v>
@@ -3274,15 +3273,15 @@
         <v>1992</v>
       </c>
       <c r="G26">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="B27" t="s">
         <v>137</v>
@@ -3300,10 +3299,10 @@
         <v>1992</v>
       </c>
       <c r="G27">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -3326,15 +3325,15 @@
         <v>1992</v>
       </c>
       <c r="G28">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="B29" t="s">
         <v>137</v>
@@ -3352,15 +3351,15 @@
         <v>1992</v>
       </c>
       <c r="G29">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" t="s">
         <v>137</v>
@@ -3378,19 +3377,19 @@
         <v>1992</v>
       </c>
       <c r="G30">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="H30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" t="s">
         <v>137</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="C31" t="s">
         <v>9</v>
       </c>
@@ -3401,21 +3400,21 @@
         <v>9</v>
       </c>
       <c r="F31">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="G31">
-        <v>2020</v>
-      </c>
-      <c r="H31" t="s">
-        <v>171</v>
+        <v>2009</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>170</v>
-      </c>
-      <c r="B32" t="s">
-        <v>137</v>
+        <v>171</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -3427,65 +3426,13 @@
         <v>9</v>
       </c>
       <c r="F32">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="G32">
-        <v>2020</v>
-      </c>
-      <c r="H32" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>137</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33">
-        <v>2000</v>
-      </c>
-      <c r="G33">
-        <v>2010</v>
-      </c>
-      <c r="H33" s="5" t="s">
+        <v>2008</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>173</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34">
-        <v>2000</v>
-      </c>
-      <c r="G34">
-        <v>2008</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>